<commit_message>
inventory upload template update
</commit_message>
<xml_diff>
--- a/public/templates/inventory-upload-template.xlsx
+++ b/public/templates/inventory-upload-template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B9F459-D71B-43CB-8831-92646525FAB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7199A988-6669-4081-9D8B-A5F86CDFE7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21450" yWindow="0" windowWidth="21555" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>MAIN</t>
   </si>
   <si>
-    <t>VAN-001</t>
-  </si>
-  <si>
-    <t>SAMPLE</t>
-  </si>
-  <si>
     <t>SKU CODE</t>
   </si>
   <si>
@@ -41,6 +35,21 @@
   </si>
   <si>
     <t>BELLIC BRIGHTENING SOAP 135gm</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>EXPIRY DATE</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>PCS</t>
   </si>
 </sst>
 </file>
@@ -95,7 +104,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,54 +385,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.5703125" style="2"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
+      <c r="F2" s="2">
+        <v>46188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>